<commit_message>
Finished NODE-CNN runs for 3 sets of NODEs
</commit_message>
<xml_diff>
--- a/Results/Classification/Control vs Atypical/Control 0 (13, 11, 8, 14, 6)/Atypical 0 (0, 7, 12, 8, 11)/NCDE_32nodes_Control_vs_Atypical_batchsize3_200maxITER_None_smoothing0_dropout0.0.xlsx
+++ b/Results/Classification/Control vs Atypical/Control 0 (13, 11, 8, 14, 6)/Atypical 0 (0, 7, 12, 8, 11)/NCDE_32nodes_Control_vs_Atypical_batchsize3_200maxITER_None_smoothing0_dropout0.0.xlsx
@@ -456,10 +456,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.8824145423368052</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.8824145423368052</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -470,10 +470,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.8769092692153508</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.8769092692153508</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -484,10 +484,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.6703762919267402</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.6703762919267402</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -495,13 +495,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.2752038298194512</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.2752038298194512</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -509,13 +509,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.07237308967002483</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.07237308967002483</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -523,13 +523,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.03241780870271954</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.9675821912972804</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -537,13 +537,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.3240371710350318</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.6759628289649682</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -554,10 +554,10 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.5446593746588304</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.4553406253411696</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -568,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.6639029842498251</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.3360970157501749</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -579,19 +579,19 @@
         <v>15</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.3342725366030656</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.6657274633969344</v>
       </c>
       <c r="F11">
-        <v>20.64662742614746</v>
+        <v>1.241117358207703</v>
       </c>
       <c r="G11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -605,10 +605,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.9717628801031348</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.9717628801031348</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -619,10 +619,10 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0.9403129537294537</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0.9403129537294537</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -633,10 +633,10 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.8192659231572341</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0.8192659231572341</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -644,13 +644,13 @@
         <v>9</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.2601880179357907</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0.2601880179357907</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -658,13 +658,13 @@
         <v>10</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0.03002036616483027</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.03002036616483027</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -672,13 +672,13 @@
         <v>11</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0.00677333948388859</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.9932266605161114</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -686,13 +686,13 @@
         <v>12</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0.2648327109808429</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.7351672890191571</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -703,10 +703,10 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0.6341751954120193</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.3658248045879807</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -717,10 +717,10 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0.6949513306309474</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.3050486693690526</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -728,19 +728,19 @@
         <v>15</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.3260708628823657</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.6739291371176344</v>
       </c>
       <c r="F21">
-        <v>27.29671096801758</v>
+        <v>1.669172644615173</v>
       </c>
       <c r="G21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>